<commit_message>
Finalizada tarea de Taller Semana 8
</commit_message>
<xml_diff>
--- a/Semana 8/Taller Smana 8.xlsx
+++ b/Semana 8/Taller Smana 8.xlsx
@@ -1,23 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\megam\Unitec\Ing. en Sistemas\metodologiadelainvestigacion\Semana 8\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcellomenjivarmontesdeoca/Documents/Unitec/metodologiadelainvestigacion/Semana 8/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EEA7846-5141-4ED2-9716-650B44FC28B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D21BD580-6823-8748-A48A-63C0D71FE51C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{96F26AA6-DAFA-4E79-BB74-3FAABF4F0554}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{96F26AA6-DAFA-4E79-BB74-3FAABF4F0554}"/>
   </bookViews>
   <sheets>
     <sheet name="Portada" sheetId="2" r:id="rId1"/>
     <sheet name="Tabla" sheetId="1" r:id="rId2"/>
     <sheet name="1. Género" sheetId="3" r:id="rId3"/>
     <sheet name="2. Música Preferida " sheetId="4" r:id="rId4"/>
+    <sheet name="3. Mes de Cumpleaños" sheetId="5" r:id="rId5"/>
+    <sheet name="4. Talla de Zapatos" sheetId="6" r:id="rId6"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v2.0" hidden="1">'2. Música Preferida '!$B$5:$B$9</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">'2. Música Preferida '!$C$4</definedName>
+    <definedName name="_xlchart.v2.2" hidden="1">'2. Música Preferida '!$C$5:$C$9</definedName>
+    <definedName name="_xlchart.v2.3" hidden="1">'2. Música Preferida '!$D$4</definedName>
+    <definedName name="_xlchart.v2.4" hidden="1">'2. Música Preferida '!$D$5:$D$9</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="113">
   <si>
     <t>Música Preferida</t>
   </si>
@@ -152,13 +161,283 @@
   </si>
   <si>
     <t>La moda del curso es de género másculino con un porcentaje de 61%</t>
+  </si>
+  <si>
+    <t>Enero</t>
+  </si>
+  <si>
+    <t>Febrero</t>
+  </si>
+  <si>
+    <t>Mes de cumpleaños</t>
+  </si>
+  <si>
+    <t>Marzo</t>
+  </si>
+  <si>
+    <t>Abril</t>
+  </si>
+  <si>
+    <t>Mayo</t>
+  </si>
+  <si>
+    <t>Junio</t>
+  </si>
+  <si>
+    <t>Julio</t>
+  </si>
+  <si>
+    <t>Agosto</t>
+  </si>
+  <si>
+    <t>Septiembre</t>
+  </si>
+  <si>
+    <t>Ocutbre</t>
+  </si>
+  <si>
+    <t>Noviembre</t>
+  </si>
+  <si>
+    <t>Diciembre</t>
+  </si>
+  <si>
+    <t>% de Frecuencia</t>
+  </si>
+  <si>
+    <t>Barra</t>
+  </si>
+  <si>
+    <t>La moda del curso es de Enero  con un porcentaje de 22.22%
+Los meses de Febrero, Marzo, Junio no tiene cumpleañeros.</t>
+  </si>
+  <si>
+    <t>MODA</t>
+  </si>
+  <si>
+    <t>Histograma</t>
+  </si>
+  <si>
+    <t>TODAS</t>
+  </si>
+  <si>
+    <t>Pastel</t>
+  </si>
+  <si>
+    <t>Talla de Zapatos</t>
+  </si>
+  <si>
+    <t>Peso</t>
+  </si>
+  <si>
+    <t>Carlo</t>
+  </si>
+  <si>
+    <t>Raul</t>
+  </si>
+  <si>
+    <t>Maria Jose</t>
+  </si>
+  <si>
+    <t>Emily</t>
+  </si>
+  <si>
+    <t>Valeria</t>
+  </si>
+  <si>
+    <t>Juan</t>
+  </si>
+  <si>
+    <t>Andrea</t>
+  </si>
+  <si>
+    <t>Diego</t>
+  </si>
+  <si>
+    <t>Rafael</t>
+  </si>
+  <si>
+    <t>Katherine</t>
+  </si>
+  <si>
+    <t>Fernando</t>
+  </si>
+  <si>
+    <t>Jesus</t>
+  </si>
+  <si>
+    <t>Astrid</t>
+  </si>
+  <si>
+    <t>Gerson</t>
+  </si>
+  <si>
+    <t>Isaul</t>
+  </si>
+  <si>
+    <t>Anthony</t>
+  </si>
+  <si>
+    <t>Stephanie</t>
+  </si>
+  <si>
+    <t>UNIVERSIDAD TECNOLÓGICA CENTROAMERICANA</t>
+  </si>
+  <si>
+    <r>
+      <t>194 - Metodología de la Investigación</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>Dra. Nelly Jeannette Alcántara Galdámez </t>
+  </si>
+  <si>
+    <r>
+      <t>Tema:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PRESENTADO POR:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>20551123 Carlo Marcello Menjivar Montes de Oca </t>
+  </si>
+  <si>
+    <r>
+      <t>CAMPUS SAN PEDRO SULA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Clase # Intervalo</t>
+  </si>
+  <si>
+    <t>Tabla de frecuencia</t>
+  </si>
+  <si>
+    <t>Limite Inferior</t>
+  </si>
+  <si>
+    <t>Limite Superior</t>
+  </si>
+  <si>
+    <t>Punto Medio</t>
+  </si>
+  <si>
+    <t>% Frec Rel</t>
+  </si>
+  <si>
+    <t>% Frec Acum</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Standard Error</t>
+  </si>
+  <si>
+    <t>Median</t>
+  </si>
+  <si>
+    <t>Mode</t>
+  </si>
+  <si>
+    <t>Standard Deviation</t>
+  </si>
+  <si>
+    <t>Sample Variance</t>
+  </si>
+  <si>
+    <t>Kurtosis</t>
+  </si>
+  <si>
+    <t>Skewness</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>Minimum</t>
+  </si>
+  <si>
+    <t>Maximum</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t># Clases</t>
+  </si>
+  <si>
+    <t>POP</t>
+  </si>
+  <si>
+    <t>Otro</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> :(</t>
+  </si>
+  <si>
+    <t>La moda del curso es el  género musical Regueton  con un porcentaje de 36%</t>
+  </si>
+  <si>
+    <t>Taller Práctico - Estadística</t>
+  </si>
+  <si>
+    <t>14 de Marzo de 2022</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,8 +460,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -207,8 +507,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -216,12 +522,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -244,12 +570,65 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="6"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="6"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="15"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -349,7 +728,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-HN"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -453,6 +832,11 @@
               </a:effectLst>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-0567-DF45-B5FB-919C17E745FE}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -496,6 +880,11 @@
               </a:effectLst>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-0567-DF45-B5FB-919C17E745FE}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -523,7 +912,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="en-HN"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -631,7 +1020,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-HN"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -679,7 +1068,1214 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-HN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Géneros músicales</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-HN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg2">
+            <a:lumMod val="75000"/>
+            <a:alpha val="27000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2. Música Preferida '!$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Frecuencia</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:alpha val="88000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+            <a:scene3d>
+              <a:camera prst="orthographicFront"/>
+              <a:lightRig rig="threePt" dir="t"/>
+            </a:scene3d>
+            <a:sp3d prstMaterial="flat">
+              <a:contourClr>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:contourClr>
+            </a:sp3d>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:alpha val="30000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:alpha val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="63500" dist="88900" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-HN"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2. Música Preferida '!$B$5:$B$9</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Regueton</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>POP</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Bachata</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Rock</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Otro</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2. Música Preferida '!$C$5:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-53BF-0C42-862E-2951350A712F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2. Música Preferida '!$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>% frec</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:alpha val="88000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+            <a:scene3d>
+              <a:camera prst="orthographicFront"/>
+              <a:lightRig rig="threePt" dir="t"/>
+            </a:scene3d>
+            <a:sp3d prstMaterial="flat">
+              <a:contourClr>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:contourClr>
+            </a:sp3d>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:alpha val="30000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:alpha val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="63500" dist="88900" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-HN"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2. Música Preferida '!$B$5:$B$9</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Regueton</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>POP</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Bachata</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Rock</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Otro</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2. Música Preferida '!$D$5:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.35714285714285715</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.21428571428571427</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.21428571428571427</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.1428571428571425E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.14285714285714285</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-53BF-0C42-862E-2951350A712F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="84"/>
+        <c:gapDepth val="53"/>
+        <c:shape val="box"/>
+        <c:axId val="15983760"/>
+        <c:axId val="15793648"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="15983760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-HN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="15793648"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="15793648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="15983760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-HN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:tint val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-HN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-HN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'3. Mes de Cumpleaños'!$C$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Frecuencia</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'3. Mes de Cumpleaños'!$B$7:$B$18</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Enero</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Febrero</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Marzo</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Abril</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Mayo</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Junio</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Julio</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Agosto</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Septiembre</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Ocutbre</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Noviembre</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Diciembre</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'3. Mes de Cumpleaños'!$C$7:$C$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F06E-8B4B-9426-706995887BBB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="100503935"/>
+        <c:axId val="2128694896"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'3. Mes de Cumpleaños'!$D$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>% de Frecuencia</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'3. Mes de Cumpleaños'!$B$7:$B$18</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Enero</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Febrero</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Marzo</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Abril</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Mayo</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Junio</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Julio</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Agosto</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Septiembre</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Ocutbre</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Noviembre</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Diciembre</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'3. Mes de Cumpleaños'!$D$7:$D$18</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.22222222222222221</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.16666666666666666</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.1111111111111111</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.5555555555555552E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.5555555555555552E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.16666666666666666</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.5555555555555552E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.5555555555555552E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.1111111111111111</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F06E-8B4B-9426-706995887BBB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="437725119"/>
+        <c:axId val="540457071"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="100503935"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-HN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2128694896"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2128694896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-HN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="100503935"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="540457071"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-HN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="437725119"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="437725119"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="540457071"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-HN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-HN"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -730,6 +2326,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="268">
   <cs:axisTitle>
@@ -1226,7 +2902,1132 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="291">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:tint val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="30000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+      <a:effectLst>
+        <a:outerShdw blurRad="63500" dist="88900" dir="2700000" algn="tl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="30000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+      <a:effectLst>
+        <a:outerShdw blurRad="63500" dist="88900" dir="2700000" algn="tl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="88000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="88000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+      <a:scene3d>
+        <a:camera prst="orthographicFront"/>
+        <a:lightRig rig="threePt" dir="t"/>
+      </a:scene3d>
+      <a:sp3d prstMaterial="flat"/>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg2">
+          <a:lumMod val="75000"/>
+          <a:alpha val="27000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:sp3d/>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="0" kern="1200" cap="all" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:sp3d/>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="328">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="95000"/>
+              <a:lumOff val="5000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="75000"/>
+              <a:lumOff val="25000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+      </a:gradFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="85000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+      </a:gradFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>177801</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>101601</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 4" descr="A picture containing icon&#10;&#10;Description automatically generated">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0A16A8A-5F7E-A341-80E3-B1E09FFBA9DA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="139700" y="177801"/>
+          <a:ext cx="2387600" cy="736600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1267,20 +4068,20 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3175</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>139452</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>38898</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1302,14 +4103,91 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6886575" y="676275"/>
-          <a:ext cx="3616077" cy="4219575"/>
+          <a:off x="676275" y="4140200"/>
+          <a:ext cx="3579023" cy="3778250"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>654050</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63FB5DAE-0673-FB48-9EF1-A824CCD79751}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>425450</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC32247A-E9FE-8942-B517-6F93205F8865}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1612,13 +4490,263 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E53FB0B-F8F5-44CB-9804-1152B11ED216}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="24"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+    </row>
+    <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+    </row>
+    <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="24"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+    </row>
+    <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="24"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+    </row>
+    <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="24"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+    </row>
+    <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+    </row>
+    <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="27"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+    </row>
+    <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="27"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+    </row>
+    <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="27"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+    </row>
+    <row r="10" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+    </row>
+    <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+    </row>
+    <row r="12" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="28"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+    </row>
+    <row r="13" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+    </row>
+    <row r="14" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="27"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+    </row>
+    <row r="15" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+    </row>
+    <row r="16" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="27"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+    </row>
+    <row r="17" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+    </row>
+    <row r="18" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="29"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+    </row>
+    <row r="19" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+    </row>
+    <row r="20" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="28"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
+    </row>
+    <row r="21" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="28"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+    </row>
+    <row r="22" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="28"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="25"/>
+    </row>
+    <row r="23" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="28"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="25"/>
+    </row>
+    <row r="24" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="B24" s="25"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+    </row>
+    <row r="25" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="B25" s="25"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A6:G6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1626,21 +4754,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14DFEDCA-794D-4211-B8AA-B0F7602EB896}">
   <dimension ref="A2:I8"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" customWidth="1"/>
+    <col min="1" max="1" width="5.5" customWidth="1"/>
+    <col min="2" max="2" width="24.1640625" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" customWidth="1"/>
-    <col min="5" max="5" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.83203125" customWidth="1"/>
+    <col min="5" max="5" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -1660,7 +4788,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1670,11 +4798,17 @@
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -1684,14 +4818,20 @@
       <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="I4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1701,14 +4841,20 @@
       <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="I5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -1718,14 +4864,20 @@
       <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="I6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1735,14 +4887,20 @@
       <c r="C7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="I7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -1752,9 +4910,15 @@
       <c r="C8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="I8" t="s">
         <v>20</v>
       </c>
@@ -1769,24 +4933,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD13F4B9-9AD9-4AE3-AF04-ABE660F19C5A}">
   <dimension ref="B2:J17"/>
   <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D6"/>
+    <sheetView zoomScale="119" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14:J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="7" t="s">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1797,7 +4961,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>22</v>
       </c>
@@ -1809,7 +4973,7 @@
         <v>0.61111111111111116</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>23</v>
       </c>
@@ -1821,7 +4985,7 @@
         <v>0.3888888888888889</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
         <v>25</v>
       </c>
@@ -1834,13 +4998,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="7" t="s">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B9" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="7"/>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C9" s="8"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>28</v>
       </c>
@@ -1848,7 +5012,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>29</v>
       </c>
@@ -1856,7 +5020,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>30</v>
       </c>
@@ -1864,20 +5028,20 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="7" t="s">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B14" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="7"/>
-      <c r="F14" s="8" t="s">
+      <c r="C14" s="8"/>
+      <c r="F14" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>32</v>
       </c>
@@ -1895,7 +5059,7 @@
       <c r="I15" s="9"/>
       <c r="J15" s="9"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
         <v>33</v>
       </c>
@@ -1908,7 +5072,7 @@
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>34</v>
       </c>
@@ -1931,75 +5095,1090 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5221DCA0-4D30-4F56-9B07-88623320FE24}">
-  <dimension ref="B3:D10"/>
+  <dimension ref="B3:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F30" sqref="F30:J32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B4" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="23" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="4"/>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="5"/>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="2">
+        <v>5</v>
+      </c>
+      <c r="D5" s="4">
+        <f>C5/$C$10</f>
+        <v>0.35714285714285715</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B6" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" s="1">
+        <v>3</v>
+      </c>
+      <c r="D6" s="5">
+        <f t="shared" ref="D6:D9" si="0">C6/$C$10</f>
+        <v>0.21428571428571427</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="2">
+        <v>3</v>
+      </c>
+      <c r="D7" s="4">
+        <f t="shared" si="0"/>
+        <v>0.21428571428571427</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="5">
+        <f t="shared" si="0"/>
+        <v>7.1428571428571425E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" s="2">
+        <v>2</v>
+      </c>
+      <c r="D9" s="4">
+        <f t="shared" si="0"/>
+        <v>0.14285714285714285</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C10" s="3">
-        <f>SUM(C8:C9)</f>
-        <v>0</v>
+        <f>SUM(C5:C9)</f>
+        <v>14</v>
       </c>
       <c r="D10" s="6">
-        <f>SUM(D8:D9)</f>
-        <v>0</v>
-      </c>
+        <f>SUM(D5:D9)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="8"/>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B17" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="8"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B19" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="F30" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="F31" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="5">
     <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="F30:J30"/>
+    <mergeCell ref="F31:J32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A8BD2D1-9D70-804F-9547-99F87E396B13}">
+  <dimension ref="B5:K36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B6" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="31">
+        <v>4</v>
+      </c>
+      <c r="D7" s="32">
+        <f>C7/$C$19</f>
+        <v>0.22222222222222221</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B8" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="33">
+        <v>0</v>
+      </c>
+      <c r="D8" s="34">
+        <f t="shared" ref="D8:D18" si="0">C8/$C$19</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="31">
+        <v>0</v>
+      </c>
+      <c r="D9" s="32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B10" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="33">
+        <v>3</v>
+      </c>
+      <c r="D10" s="34">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B11" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="31">
+        <v>2</v>
+      </c>
+      <c r="D11" s="32">
+        <f t="shared" si="0"/>
+        <v>0.1111111111111111</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="33">
+        <v>0</v>
+      </c>
+      <c r="D12" s="34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B13" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="31">
+        <v>1</v>
+      </c>
+      <c r="D13" s="32">
+        <f t="shared" si="0"/>
+        <v>5.5555555555555552E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B14" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="33">
+        <v>1</v>
+      </c>
+      <c r="D14" s="34">
+        <f t="shared" si="0"/>
+        <v>5.5555555555555552E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B15" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="31">
+        <v>3</v>
+      </c>
+      <c r="D15" s="32">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B16" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="33">
+        <v>1</v>
+      </c>
+      <c r="D16" s="34">
+        <f t="shared" si="0"/>
+        <v>5.5555555555555552E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B17" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="31">
+        <v>1</v>
+      </c>
+      <c r="D17" s="32">
+        <f t="shared" si="0"/>
+        <v>5.5555555555555552E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B18" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="33">
+        <v>2</v>
+      </c>
+      <c r="D18" s="34">
+        <f t="shared" si="0"/>
+        <v>0.1111111111111111</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B19" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="35">
+        <f>SUM(C7:C18)</f>
+        <v>18</v>
+      </c>
+      <c r="D19" s="36">
+        <f>C19/$C$19</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B22" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="8"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B24" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B27" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="8"/>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B29" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B30" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="G31" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
+    </row>
+    <row r="32" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G32" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="H32" s="15"/>
+      <c r="I32" s="15"/>
+      <c r="J32" s="15"/>
+      <c r="K32" s="15"/>
+    </row>
+    <row r="33" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="15"/>
+      <c r="K33" s="15"/>
+    </row>
+    <row r="34" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G34" s="15"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="15"/>
+      <c r="K34" s="15"/>
+    </row>
+    <row r="35" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="15"/>
+    </row>
+    <row r="36" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G36" s="15"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="15"/>
+      <c r="K36" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="G31:K31"/>
+    <mergeCell ref="G32:K36"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57564037-4983-4F43-B32E-66DF5F058255}">
+  <dimension ref="C6:N41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K9" sqref="K9:K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" customWidth="1"/>
+    <col min="10" max="10" width="15" customWidth="1"/>
+    <col min="11" max="11" width="16.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C6" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7">
+        <v>9</v>
+      </c>
+      <c r="E7">
+        <v>34</v>
+      </c>
+      <c r="F7">
+        <v>135</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+    </row>
+    <row r="8" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8">
+        <v>9</v>
+      </c>
+      <c r="E8">
+        <v>18</v>
+      </c>
+      <c r="F8">
+        <v>135</v>
+      </c>
+      <c r="H8" t="s">
+        <v>85</v>
+      </c>
+      <c r="I8" t="s">
+        <v>87</v>
+      </c>
+      <c r="J8" t="s">
+        <v>88</v>
+      </c>
+      <c r="K8" t="s">
+        <v>89</v>
+      </c>
+      <c r="L8" t="s">
+        <v>24</v>
+      </c>
+      <c r="M8" t="s">
+        <v>90</v>
+      </c>
+      <c r="N8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9">
+        <v>7.5</v>
+      </c>
+      <c r="E9">
+        <v>21</v>
+      </c>
+      <c r="F9">
+        <v>132</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <f>D38</f>
+        <v>6</v>
+      </c>
+      <c r="J9" s="21">
+        <f>I9+$G$38</f>
+        <v>7.125</v>
+      </c>
+      <c r="K9">
+        <f>(J9+I9)/2</f>
+        <v>6.5625</v>
+      </c>
+    </row>
+    <row r="10" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10">
+        <v>6</v>
+      </c>
+      <c r="E10">
+        <v>17</v>
+      </c>
+      <c r="F10">
+        <v>137</v>
+      </c>
+      <c r="H10">
+        <v>2</v>
+      </c>
+      <c r="I10" s="21">
+        <f>J9</f>
+        <v>7.125</v>
+      </c>
+      <c r="J10" s="21">
+        <f>I10+$G$38</f>
+        <v>8.25</v>
+      </c>
+      <c r="K10">
+        <f t="shared" ref="K10:K12" si="0">(J10+I10)/2</f>
+        <v>7.6875</v>
+      </c>
+    </row>
+    <row r="11" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11">
+        <v>6.5</v>
+      </c>
+      <c r="E11">
+        <v>21</v>
+      </c>
+      <c r="F11">
+        <v>120</v>
+      </c>
+      <c r="H11">
+        <v>3</v>
+      </c>
+      <c r="I11" s="21">
+        <f t="shared" ref="I11:I12" si="1">J10</f>
+        <v>8.25</v>
+      </c>
+      <c r="J11" s="21">
+        <f t="shared" ref="J11:J12" si="2">I11+$G$38</f>
+        <v>9.375</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="0"/>
+        <v>8.8125</v>
+      </c>
+    </row>
+    <row r="12" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12">
+        <v>7</v>
+      </c>
+      <c r="E12">
+        <v>17</v>
+      </c>
+      <c r="F12">
+        <v>115</v>
+      </c>
+      <c r="H12">
+        <v>4</v>
+      </c>
+      <c r="I12" s="21">
+        <f t="shared" si="1"/>
+        <v>9.375</v>
+      </c>
+      <c r="J12" s="21">
+        <f t="shared" si="2"/>
+        <v>10.5</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="0"/>
+        <v>9.9375</v>
+      </c>
+    </row>
+    <row r="13" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13">
+        <v>7.5</v>
+      </c>
+      <c r="E13">
+        <v>19</v>
+      </c>
+      <c r="F13">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14">
+        <v>8.5</v>
+      </c>
+      <c r="E14">
+        <v>17</v>
+      </c>
+      <c r="F14">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15">
+        <v>10</v>
+      </c>
+      <c r="E15">
+        <v>19</v>
+      </c>
+      <c r="F15">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="16" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16">
+        <v>9</v>
+      </c>
+      <c r="E16">
+        <v>18</v>
+      </c>
+      <c r="F16">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17">
+        <v>8</v>
+      </c>
+      <c r="E17">
+        <v>18</v>
+      </c>
+      <c r="F17">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18">
+        <v>10.5</v>
+      </c>
+      <c r="E18">
+        <v>19</v>
+      </c>
+      <c r="F18">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>72</v>
+      </c>
+      <c r="D19">
+        <v>8</v>
+      </c>
+      <c r="E19">
+        <v>17</v>
+      </c>
+      <c r="F19">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20">
+        <v>10</v>
+      </c>
+      <c r="E20">
+        <v>18</v>
+      </c>
+      <c r="F20">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>73</v>
+      </c>
+      <c r="D21">
+        <v>9</v>
+      </c>
+      <c r="E21">
+        <v>19</v>
+      </c>
+      <c r="F21">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D22">
+        <v>8</v>
+      </c>
+      <c r="E22">
+        <v>18</v>
+      </c>
+      <c r="F22">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="23" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23">
+        <v>9</v>
+      </c>
+      <c r="E23">
+        <v>17</v>
+      </c>
+      <c r="F23">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="24" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
+        <v>75</v>
+      </c>
+      <c r="D24">
+        <v>9.5</v>
+      </c>
+      <c r="E24">
+        <v>18</v>
+      </c>
+      <c r="F24">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="25" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
+        <v>76</v>
+      </c>
+      <c r="D25">
+        <v>7</v>
+      </c>
+      <c r="E25">
+        <v>19</v>
+      </c>
+      <c r="F25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="26" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C27" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D27" s="18"/>
+      <c r="F27" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G27" s="8"/>
+    </row>
+    <row r="28" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="F28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G28" s="19">
+        <f>D29</f>
+        <v>8.3684210526315788</v>
+      </c>
+    </row>
+    <row r="29" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C29" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="D29" s="16">
+        <v>8.3684210526315788</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G29" s="2">
+        <f>D31</f>
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="30" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C30" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="D30" s="16">
+        <v>0.28572802587547952</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G30" s="1">
+        <f>D32</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C31" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="D31" s="16">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="32" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C32" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="D32" s="16">
+        <v>9</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G32" s="8"/>
+    </row>
+    <row r="33" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C33" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="D33" s="16">
+        <v>1.2454595901285901</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G33" s="1">
+        <f>D37</f>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="34" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C34" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="D34" s="16">
+        <v>1.5511695906432754</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G34" s="20">
+        <f>D33</f>
+        <v>1.2454595901285901</v>
+      </c>
+    </row>
+    <row r="35" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C35" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="D35" s="16">
+        <v>-0.69906045051283972</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G35" s="19">
+        <f>D34</f>
+        <v>1.5511695906432754</v>
+      </c>
+    </row>
+    <row r="36" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C36" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="D36" s="16">
+        <v>-0.17067038264105736</v>
+      </c>
+    </row>
+    <row r="37" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C37" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="D37" s="16">
+        <v>4.5</v>
+      </c>
+      <c r="F37" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="38" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C38" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="D38" s="16">
+        <v>6</v>
+      </c>
+      <c r="F38" s="22">
+        <f>ROUND(SQRT(D41),0)</f>
+        <v>4</v>
+      </c>
+      <c r="G38" s="21">
+        <f>D37/F38</f>
+        <v>1.125</v>
+      </c>
+    </row>
+    <row r="39" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C39" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="D39" s="16">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="40" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C40" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="D40" s="16">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="41" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C41" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D41" s="17">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="H7:N7"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F32:G32"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fin de taller semana 9
</commit_message>
<xml_diff>
--- a/Semana 8/Taller Smana 8.xlsx
+++ b/Semana 8/Taller Smana 8.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shello\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcellomenjivarmontesdeoca/Documents/Unitec/metodologiadelainvestigacion/Semana 8/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB7714DB-560A-4D74-AACB-B7212740375F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E2BF25C-A741-C54A-9E94-B209015F563F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14040" activeTab="7" xr2:uid="{96F26AA6-DAFA-4E79-BB74-3FAABF4F0554}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="6" xr2:uid="{96F26AA6-DAFA-4E79-BB74-3FAABF4F0554}"/>
   </bookViews>
   <sheets>
     <sheet name="Portada" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="132">
   <si>
     <t>Música Preferida</t>
   </si>
@@ -611,7 +611,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -692,6 +692,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -810,7 +813,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-HN"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -994,7 +997,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="en-HN"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -1102,7 +1105,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-HN"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1150,7 +1153,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-HN"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1220,7 +1223,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-HN"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1355,7 +1358,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="en-HN"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -1517,7 +1520,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="en-HN"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -1648,7 +1651,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-HN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="15793648"/>
@@ -1707,7 +1710,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-HN"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1746,7 +1749,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-HN"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1803,7 +1806,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-HN"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2159,7 +2162,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-HN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2128694896"/>
@@ -2217,7 +2220,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-HN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="100503935"/>
@@ -2258,7 +2261,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-HN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="437725119"/>
@@ -2317,7 +2320,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-HN"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2358,7 +2361,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-HN"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2671,7 +2674,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-HN"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2736,7 +2739,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="en-HN"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -2922,7 +2925,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-HN"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2953,7 +2956,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-HN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="363446032"/>
@@ -3044,7 +3047,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-HN"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3075,7 +3078,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-HN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="363426480"/>
@@ -3116,7 +3119,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-HN"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3156,7 +3159,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-HN"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3215,6 +3218,10 @@
           <cx:layoutPr>
             <cx:binning intervalClosed="r"/>
           </cx:layoutPr>
+          <cx:axisId val="1"/>
+        </cx:series>
+        <cx:series layoutId="paretoLine" ownerIdx="0" uniqueId="{7EC8E164-5C75-2741-97BD-6C6076FE94EF}">
+          <cx:axisId val="2"/>
         </cx:series>
       </cx:plotAreaRegion>
       <cx:axis id="0">
@@ -3224,6 +3231,11 @@
       <cx:axis id="1">
         <cx:valScaling/>
         <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="2">
+        <cx:valScaling max="1" min="0"/>
+        <cx:units unit="percentage"/>
         <cx:tickLabels/>
       </cx:axis>
     </cx:plotArea>
@@ -6361,16 +6373,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>606425</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>428624</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>130174</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>301625</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>126999</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -6406,8 +6418,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="2435225" y="371475"/>
-              <a:ext cx="4572000" cy="2838450"/>
+              <a:off x="3121024" y="4562474"/>
+              <a:ext cx="7394575" cy="3616325"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -6743,9 +6755,9 @@
       <selection activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="15"/>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -6755,7 +6767,7 @@
       <c r="G1" s="16"/>
       <c r="H1" s="28"/>
     </row>
-    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -6765,7 +6777,7 @@
       <c r="G2" s="16"/>
       <c r="H2" s="28"/>
     </row>
-    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="15"/>
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
@@ -6775,7 +6787,7 @@
       <c r="G3" s="16"/>
       <c r="H3" s="28"/>
     </row>
-    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="15"/>
       <c r="B4" s="16"/>
       <c r="C4" s="16"/>
@@ -6785,7 +6797,7 @@
       <c r="G4" s="16"/>
       <c r="H4" s="28"/>
     </row>
-    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="15"/>
       <c r="B5" s="16"/>
       <c r="C5" s="16"/>
@@ -6795,19 +6807,19 @@
       <c r="G5" s="16"/>
       <c r="H5" s="28"/>
     </row>
-    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="39" t="s">
+    <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
       <c r="H6" s="28"/>
     </row>
-    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="17"/>
       <c r="B7" s="16"/>
       <c r="C7" s="16"/>
@@ -6817,7 +6829,7 @@
       <c r="G7" s="16"/>
       <c r="H7" s="28"/>
     </row>
-    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="17"/>
       <c r="B8" s="16"/>
       <c r="C8" s="16"/>
@@ -6827,7 +6839,7 @@
       <c r="G8" s="16"/>
       <c r="H8" s="28"/>
     </row>
-    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="17"/>
       <c r="B9" s="16"/>
       <c r="C9" s="16"/>
@@ -6837,7 +6849,7 @@
       <c r="G9" s="16"/>
       <c r="H9" s="28"/>
     </row>
-    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="18" t="s">
         <v>78</v>
       </c>
@@ -6849,7 +6861,7 @@
       <c r="G10" s="16"/>
       <c r="H10" s="28"/>
     </row>
-    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
         <v>79</v>
       </c>
@@ -6861,7 +6873,7 @@
       <c r="G11" s="16"/>
       <c r="H11" s="28"/>
     </row>
-    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="18"/>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
@@ -6871,7 +6883,7 @@
       <c r="G12" s="16"/>
       <c r="H12" s="28"/>
     </row>
-    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="18" t="s">
         <v>80</v>
       </c>
@@ -6883,7 +6895,7 @@
       <c r="G13" s="16"/>
       <c r="H13" s="28"/>
     </row>
-    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="17"/>
       <c r="B14" s="16"/>
       <c r="C14" s="16"/>
@@ -6893,7 +6905,7 @@
       <c r="G14" s="16"/>
       <c r="H14" s="28"/>
     </row>
-    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
         <v>111</v>
       </c>
@@ -6905,7 +6917,7 @@
       <c r="G15" s="16"/>
       <c r="H15" s="28"/>
     </row>
-    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="17"/>
       <c r="B16" s="16"/>
       <c r="C16" s="16"/>
@@ -6915,7 +6927,7 @@
       <c r="G16" s="16"/>
       <c r="H16" s="28"/>
     </row>
-    <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="18" t="s">
         <v>81</v>
       </c>
@@ -6927,7 +6939,7 @@
       <c r="G17" s="16"/>
       <c r="H17" s="28"/>
     </row>
-    <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="19"/>
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
@@ -6937,7 +6949,7 @@
       <c r="G18" s="16"/>
       <c r="H18" s="28"/>
     </row>
-    <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="19" t="s">
         <v>82</v>
       </c>
@@ -6949,7 +6961,7 @@
       <c r="G19" s="16"/>
       <c r="H19" s="28"/>
     </row>
-    <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="18"/>
       <c r="B20" s="16"/>
       <c r="C20" s="16"/>
@@ -6959,7 +6971,7 @@
       <c r="G20" s="16"/>
       <c r="H20" s="28"/>
     </row>
-    <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="18"/>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
@@ -6969,7 +6981,7 @@
       <c r="G21" s="16"/>
       <c r="H21" s="28"/>
     </row>
-    <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="18"/>
       <c r="B22" s="16"/>
       <c r="C22" s="16"/>
@@ -6979,7 +6991,7 @@
       <c r="G22" s="16"/>
       <c r="H22" s="28"/>
     </row>
-    <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="18"/>
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
@@ -6989,7 +7001,7 @@
       <c r="G23" s="16"/>
       <c r="H23" s="28"/>
     </row>
-    <row r="24" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="18" t="s">
         <v>83</v>
       </c>
@@ -7001,7 +7013,7 @@
       <c r="G24" s="16"/>
       <c r="H24" s="28"/>
     </row>
-    <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="18" t="s">
         <v>112</v>
       </c>
@@ -7013,7 +7025,7 @@
       <c r="G25" s="16"/>
       <c r="H25" s="28"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="28"/>
       <c r="B26" s="28"/>
       <c r="C26" s="28"/>
@@ -7040,17 +7052,17 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" customWidth="1"/>
+    <col min="1" max="1" width="5.5" customWidth="1"/>
+    <col min="2" max="2" width="24.1640625" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" customWidth="1"/>
-    <col min="5" max="5" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.83203125" customWidth="1"/>
+    <col min="5" max="5" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -7070,7 +7082,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -7090,7 +7102,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -7113,7 +7125,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -7136,7 +7148,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -7159,7 +7171,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -7182,7 +7194,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -7219,20 +7231,20 @@
       <selection activeCell="F14" sqref="F14:J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="40" t="s">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B2" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
@@ -7243,7 +7255,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>22</v>
       </c>
@@ -7255,7 +7267,7 @@
         <v>0.61111111111111116</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>23</v>
       </c>
@@ -7267,7 +7279,7 @@
         <v>0.3888888888888889</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
         <v>25</v>
       </c>
@@ -7280,13 +7292,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="40" t="s">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B9" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="40"/>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C9" s="41"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>28</v>
       </c>
@@ -7294,7 +7306,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>29</v>
       </c>
@@ -7302,7 +7314,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>30</v>
       </c>
@@ -7310,20 +7322,20 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="40" t="s">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B14" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="40"/>
-      <c r="F14" s="42" t="s">
+      <c r="C14" s="41"/>
+      <c r="F14" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="G14" s="42"/>
-      <c r="H14" s="42"/>
-      <c r="I14" s="42"/>
-      <c r="J14" s="42"/>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="43"/>
+      <c r="J14" s="43"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>32</v>
       </c>
@@ -7333,28 +7345,28 @@
       <c r="D15" t="s">
         <v>35</v>
       </c>
-      <c r="F15" s="41" t="s">
+      <c r="F15" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="G15" s="41"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="41"/>
-      <c r="J15" s="41"/>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G15" s="42"/>
+      <c r="H15" s="42"/>
+      <c r="I15" s="42"/>
+      <c r="J15" s="42"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F16" s="41"/>
-      <c r="G16" s="41"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="41"/>
-      <c r="J16" s="41"/>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="F16" s="42"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>34</v>
       </c>
@@ -7383,21 +7395,21 @@
       <selection activeCell="F30" sqref="F30:J32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="40" t="s">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B3" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" s="14" t="s">
         <v>5</v>
       </c>
@@ -7408,7 +7420,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>16</v>
       </c>
@@ -7420,7 +7432,7 @@
         <v>0.35714285714285715</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>107</v>
       </c>
@@ -7432,7 +7444,7 @@
         <v>0.21428571428571427</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>18</v>
       </c>
@@ -7444,7 +7456,7 @@
         <v>0.21428571428571427</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>19</v>
       </c>
@@ -7456,7 +7468,7 @@
         <v>7.1428571428571425E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>108</v>
       </c>
@@ -7468,7 +7480,7 @@
         <v>0.14285714285714285</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
         <v>25</v>
       </c>
@@ -7481,13 +7493,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="40" t="s">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="40"/>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C12" s="41"/>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>28</v>
       </c>
@@ -7495,7 +7507,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>29</v>
       </c>
@@ -7503,7 +7515,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>30</v>
       </c>
@@ -7514,13 +7526,13 @@
         <v>109</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="40" t="s">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B17" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="40"/>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C17" s="41"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>32</v>
       </c>
@@ -7528,7 +7540,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
         <v>33</v>
       </c>
@@ -7536,7 +7548,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>34</v>
       </c>
@@ -7544,30 +7556,30 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F30" s="42" t="s">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="F30" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="G30" s="42"/>
-      <c r="H30" s="42"/>
-      <c r="I30" s="42"/>
-      <c r="J30" s="42"/>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F31" s="41" t="s">
+      <c r="G30" s="43"/>
+      <c r="H30" s="43"/>
+      <c r="I30" s="43"/>
+      <c r="J30" s="43"/>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="F31" s="42" t="s">
         <v>110</v>
       </c>
-      <c r="G31" s="41"/>
-      <c r="H31" s="41"/>
-      <c r="I31" s="41"/>
-      <c r="J31" s="41"/>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F32" s="41"/>
-      <c r="G32" s="41"/>
-      <c r="H32" s="41"/>
-      <c r="I32" s="41"/>
-      <c r="J32" s="41"/>
+      <c r="G31" s="42"/>
+      <c r="H31" s="42"/>
+      <c r="I31" s="42"/>
+      <c r="J31" s="42"/>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="F32" s="42"/>
+      <c r="G32" s="42"/>
+      <c r="H32" s="42"/>
+      <c r="I32" s="42"/>
+      <c r="J32" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -7590,18 +7602,18 @@
       <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" s="20" t="s">
         <v>40</v>
       </c>
@@ -7612,7 +7624,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B7" s="21" t="s">
         <v>38</v>
       </c>
@@ -7624,7 +7636,7 @@
         <v>0.22222222222222221</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B8" s="23" t="s">
         <v>39</v>
       </c>
@@ -7636,7 +7648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B9" s="21" t="s">
         <v>41</v>
       </c>
@@ -7648,7 +7660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B10" s="23" t="s">
         <v>42</v>
       </c>
@@ -7660,7 +7672,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B11" s="21" t="s">
         <v>43</v>
       </c>
@@ -7672,7 +7684,7 @@
         <v>0.1111111111111111</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B12" s="23" t="s">
         <v>44</v>
       </c>
@@ -7684,7 +7696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B13" s="21" t="s">
         <v>45</v>
       </c>
@@ -7696,7 +7708,7 @@
         <v>5.5555555555555552E-2</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B14" s="23" t="s">
         <v>46</v>
       </c>
@@ -7708,7 +7720,7 @@
         <v>5.5555555555555552E-2</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B15" s="21" t="s">
         <v>47</v>
       </c>
@@ -7720,7 +7732,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B16" s="23" t="s">
         <v>48</v>
       </c>
@@ -7732,7 +7744,7 @@
         <v>5.5555555555555552E-2</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B17" s="21" t="s">
         <v>49</v>
       </c>
@@ -7744,7 +7756,7 @@
         <v>5.5555555555555552E-2</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B18" s="23" t="s">
         <v>50</v>
       </c>
@@ -7756,7 +7768,7 @@
         <v>0.1111111111111111</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B19" s="25" t="s">
         <v>25</v>
       </c>
@@ -7769,13 +7781,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="40" t="s">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B22" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="40"/>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C22" s="41"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>28</v>
       </c>
@@ -7783,7 +7795,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
         <v>29</v>
       </c>
@@ -7791,7 +7803,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
         <v>30</v>
       </c>
@@ -7799,13 +7811,13 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="40" t="s">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B27" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="40"/>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C27" s="41"/>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
         <v>32</v>
       </c>
@@ -7816,7 +7828,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
         <v>33</v>
       </c>
@@ -7824,7 +7836,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
         <v>34</v>
       </c>
@@ -7832,51 +7844,51 @@
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="G31" s="42" t="s">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="G31" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="H31" s="42"/>
-      <c r="I31" s="42"/>
-      <c r="J31" s="42"/>
-      <c r="K31" s="42"/>
-    </row>
-    <row r="32" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G32" s="43" t="s">
+      <c r="H31" s="43"/>
+      <c r="I31" s="43"/>
+      <c r="J31" s="43"/>
+      <c r="K31" s="43"/>
+    </row>
+    <row r="32" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G32" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="H32" s="43"/>
-      <c r="I32" s="43"/>
-      <c r="J32" s="43"/>
-      <c r="K32" s="43"/>
-    </row>
-    <row r="33" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G33" s="43"/>
-      <c r="H33" s="43"/>
-      <c r="I33" s="43"/>
-      <c r="J33" s="43"/>
-      <c r="K33" s="43"/>
-    </row>
-    <row r="34" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G34" s="43"/>
-      <c r="H34" s="43"/>
-      <c r="I34" s="43"/>
-      <c r="J34" s="43"/>
-      <c r="K34" s="43"/>
-    </row>
-    <row r="35" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G35" s="43"/>
-      <c r="H35" s="43"/>
-      <c r="I35" s="43"/>
-      <c r="J35" s="43"/>
-      <c r="K35" s="43"/>
-    </row>
-    <row r="36" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G36" s="43"/>
-      <c r="H36" s="43"/>
-      <c r="I36" s="43"/>
-      <c r="J36" s="43"/>
-      <c r="K36" s="43"/>
+      <c r="H32" s="44"/>
+      <c r="I32" s="44"/>
+      <c r="J32" s="44"/>
+      <c r="K32" s="44"/>
+    </row>
+    <row r="33" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G33" s="44"/>
+      <c r="H33" s="44"/>
+      <c r="I33" s="44"/>
+      <c r="J33" s="44"/>
+      <c r="K33" s="44"/>
+    </row>
+    <row r="34" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G34" s="44"/>
+      <c r="H34" s="44"/>
+      <c r="I34" s="44"/>
+      <c r="J34" s="44"/>
+      <c r="K34" s="44"/>
+    </row>
+    <row r="35" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G35" s="44"/>
+      <c r="H35" s="44"/>
+      <c r="I35" s="44"/>
+      <c r="J35" s="44"/>
+      <c r="K35" s="44"/>
+    </row>
+    <row r="36" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G36" s="44"/>
+      <c r="H36" s="44"/>
+      <c r="I36" s="44"/>
+      <c r="J36" s="44"/>
+      <c r="K36" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -7898,24 +7910,24 @@
       <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
     <col min="10" max="10" width="15" customWidth="1"/>
-    <col min="11" max="11" width="16.28515625" customWidth="1"/>
+    <col min="11" max="11" width="16.33203125" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:13" x14ac:dyDescent="0.2">
       <c r="J1" s="34"/>
     </row>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B2" s="8" t="s">
         <v>84</v>
       </c>
@@ -7929,7 +7941,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>60</v>
       </c>
@@ -7942,17 +7954,17 @@
       <c r="E3">
         <v>135</v>
       </c>
-      <c r="G3" s="40" t="s">
+      <c r="G3" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="40"/>
-      <c r="L3" s="40"/>
-      <c r="M3" s="40"/>
-    </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="41"/>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>61</v>
       </c>
@@ -7987,7 +7999,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>62</v>
       </c>
@@ -8027,7 +8039,7 @@
         <v>0.21052631578947367</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>63</v>
       </c>
@@ -8067,7 +8079,7 @@
         <v>0.47368421052631576</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>64</v>
       </c>
@@ -8107,7 +8119,7 @@
         <v>0.78947368421052633</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>65</v>
       </c>
@@ -8147,7 +8159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>66</v>
       </c>
@@ -8172,7 +8184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>67</v>
       </c>
@@ -8186,7 +8198,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>68</v>
       </c>
@@ -8206,7 +8218,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>70</v>
       </c>
@@ -8226,7 +8238,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>69</v>
       </c>
@@ -8246,7 +8258,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>71</v>
       </c>
@@ -8266,7 +8278,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>72</v>
       </c>
@@ -8286,7 +8298,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>68</v>
       </c>
@@ -8302,7 +8314,7 @@
       <c r="H16" s="11"/>
       <c r="I16" s="11"/>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>73</v>
       </c>
@@ -8316,7 +8328,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>74</v>
       </c>
@@ -8330,7 +8342,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>67</v>
       </c>
@@ -8344,7 +8356,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>75</v>
       </c>
@@ -8358,7 +8370,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>76</v>
       </c>
@@ -8372,33 +8384,33 @@
         <v>150</v>
       </c>
     </row>
-    <row r="22" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H22" s="40" t="s">
+    <row r="22" spans="2:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H22" s="41" t="s">
         <v>124</v>
       </c>
-      <c r="I22" s="40"/>
-      <c r="J22" s="40"/>
-      <c r="K22" s="40"/>
-      <c r="L22" s="40"/>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="I22" s="41"/>
+      <c r="J22" s="41"/>
+      <c r="K22" s="41"/>
+      <c r="L22" s="41"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B23" s="31" t="s">
         <v>92</v>
       </c>
       <c r="C23" s="31"/>
-      <c r="E23" s="40" t="s">
+      <c r="E23" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="F23" s="40"/>
-      <c r="H23" s="44" t="s">
+      <c r="F23" s="41"/>
+      <c r="H23" s="45" t="s">
         <v>116</v>
       </c>
-      <c r="I23" s="44"/>
-      <c r="J23" s="44"/>
-      <c r="K23" s="44"/>
-      <c r="L23" s="44"/>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="I23" s="45"/>
+      <c r="J23" s="45"/>
+      <c r="K23" s="45"/>
+      <c r="L23" s="45"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
       <c r="E24" s="1" t="s">
@@ -8408,15 +8420,15 @@
         <f>C25</f>
         <v>8.3684210526315788</v>
       </c>
-      <c r="H24" s="44" t="s">
+      <c r="H24" s="45" t="s">
         <v>117</v>
       </c>
-      <c r="I24" s="44"/>
-      <c r="J24" s="44"/>
-      <c r="K24" s="44"/>
-      <c r="L24" s="44"/>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="I24" s="45"/>
+      <c r="J24" s="45"/>
+      <c r="K24" s="45"/>
+      <c r="L24" s="45"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B25" s="10" t="s">
         <v>93</v>
       </c>
@@ -8430,15 +8442,15 @@
         <f>C27</f>
         <v>8.5</v>
       </c>
-      <c r="H25" s="44" t="s">
+      <c r="H25" s="45" t="s">
         <v>118</v>
       </c>
-      <c r="I25" s="44"/>
-      <c r="J25" s="44"/>
-      <c r="K25" s="44"/>
-      <c r="L25" s="44"/>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="I25" s="45"/>
+      <c r="J25" s="45"/>
+      <c r="K25" s="45"/>
+      <c r="L25" s="45"/>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B26" s="10" t="s">
         <v>94</v>
       </c>
@@ -8452,49 +8464,49 @@
         <f>C28</f>
         <v>9</v>
       </c>
-      <c r="H26" s="44" t="s">
+      <c r="H26" s="45" t="s">
         <v>119</v>
       </c>
-      <c r="I26" s="44"/>
-      <c r="J26" s="44"/>
-      <c r="K26" s="44"/>
-      <c r="L26" s="44"/>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="I26" s="45"/>
+      <c r="J26" s="45"/>
+      <c r="K26" s="45"/>
+      <c r="L26" s="45"/>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B27" s="10" t="s">
         <v>95</v>
       </c>
       <c r="C27" s="10">
         <v>8.5</v>
       </c>
-      <c r="H27" s="44" t="s">
+      <c r="H27" s="45" t="s">
         <v>120</v>
       </c>
-      <c r="I27" s="44"/>
-      <c r="J27" s="44"/>
-      <c r="K27" s="44"/>
-      <c r="L27" s="44"/>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="I27" s="45"/>
+      <c r="J27" s="45"/>
+      <c r="K27" s="45"/>
+      <c r="L27" s="45"/>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B28" s="10" t="s">
         <v>96</v>
       </c>
       <c r="C28" s="10">
         <v>9</v>
       </c>
-      <c r="E28" s="40" t="s">
+      <c r="E28" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="F28" s="40"/>
-      <c r="H28" s="44" t="s">
+      <c r="F28" s="41"/>
+      <c r="H28" s="45" t="s">
         <v>121</v>
       </c>
-      <c r="I28" s="44"/>
-      <c r="J28" s="44"/>
-      <c r="K28" s="44"/>
-      <c r="L28" s="44"/>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="I28" s="45"/>
+      <c r="J28" s="45"/>
+      <c r="K28" s="45"/>
+      <c r="L28" s="45"/>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B29" s="10" t="s">
         <v>97</v>
       </c>
@@ -8508,15 +8520,15 @@
         <f>C33</f>
         <v>4.5</v>
       </c>
-      <c r="H29" s="44" t="s">
+      <c r="H29" s="45" t="s">
         <v>123</v>
       </c>
-      <c r="I29" s="44"/>
-      <c r="J29" s="44"/>
-      <c r="K29" s="44"/>
-      <c r="L29" s="44"/>
-    </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="I29" s="45"/>
+      <c r="J29" s="45"/>
+      <c r="K29" s="45"/>
+      <c r="L29" s="45"/>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B30" s="10" t="s">
         <v>98</v>
       </c>
@@ -8530,15 +8542,15 @@
         <f>C29</f>
         <v>1.2454595901285901</v>
       </c>
-      <c r="H30" s="44" t="s">
+      <c r="H30" s="45" t="s">
         <v>122</v>
       </c>
-      <c r="I30" s="44"/>
-      <c r="J30" s="44"/>
-      <c r="K30" s="44"/>
-      <c r="L30" s="44"/>
-    </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
+      <c r="K30" s="45"/>
+      <c r="L30" s="45"/>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B31" s="10" t="s">
         <v>99</v>
       </c>
@@ -8553,7 +8565,7 @@
         <v>1.5511695906432754</v>
       </c>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B32" s="10" t="s">
         <v>100</v>
       </c>
@@ -8561,7 +8573,7 @@
         <v>-0.17067038264105736</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B33" s="10" t="s">
         <v>101</v>
       </c>
@@ -8575,7 +8587,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B34" s="10" t="s">
         <v>102</v>
       </c>
@@ -8591,7 +8603,7 @@
         <v>1.125</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B35" s="10" t="s">
         <v>103</v>
       </c>
@@ -8599,7 +8611,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B36" s="10" t="s">
         <v>104</v>
       </c>
@@ -8607,7 +8619,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="37" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B37" s="11" t="s">
         <v>105</v>
       </c>
@@ -8643,22 +8655,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08B977C9-52B6-46FE-AEC7-6018640403E8}">
   <dimension ref="B2:R32"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26:L26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3:R9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" customWidth="1"/>
+    <col min="6" max="6" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="27" t="s">
         <v>84</v>
       </c>
@@ -8666,7 +8678,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>60</v>
       </c>
@@ -8677,21 +8689,21 @@
         <v>92</v>
       </c>
       <c r="G3" s="38"/>
-      <c r="I3" s="40" t="s">
+      <c r="I3" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="J3" s="40"/>
-      <c r="L3" s="40" t="s">
+      <c r="J3" s="41"/>
+      <c r="L3" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="M3" s="40"/>
-      <c r="N3" s="40"/>
-      <c r="O3" s="40"/>
-      <c r="P3" s="40"/>
-      <c r="Q3" s="40"/>
-      <c r="R3" s="40"/>
-    </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="M3" s="41"/>
+      <c r="N3" s="41"/>
+      <c r="O3" s="41"/>
+      <c r="P3" s="41"/>
+      <c r="Q3" s="41"/>
+      <c r="R3" s="41"/>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>61</v>
       </c>
@@ -8729,7 +8741,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>62</v>
       </c>
@@ -8776,7 +8788,7 @@
         <v>0.94736842105263153</v>
       </c>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>63</v>
       </c>
@@ -8823,7 +8835,7 @@
         <v>0.94736842105263153</v>
       </c>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>64</v>
       </c>
@@ -8863,7 +8875,7 @@
         <v>0.94736842105263153</v>
       </c>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>65</v>
       </c>
@@ -8876,10 +8888,10 @@
       <c r="G8" s="10">
         <v>18</v>
       </c>
-      <c r="I8" s="40" t="s">
+      <c r="I8" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="J8" s="40"/>
+      <c r="J8" s="41"/>
       <c r="L8" s="21">
         <v>4</v>
       </c>
@@ -8907,7 +8919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>66</v>
       </c>
@@ -8939,7 +8951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>67</v>
       </c>
@@ -8960,7 +8972,7 @@
         <v>3.7897985565746346</v>
       </c>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>68</v>
       </c>
@@ -8981,7 +8993,7 @@
         <v>14.362573099415183</v>
       </c>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>70</v>
       </c>
@@ -8995,7 +9007,7 @@
         <v>3.6759708246004914</v>
       </c>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>69</v>
       </c>
@@ -9015,7 +9027,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>71</v>
       </c>
@@ -9037,7 +9049,7 @@
         <v>4.25</v>
       </c>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>72</v>
       </c>
@@ -9051,7 +9063,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>68</v>
       </c>
@@ -9065,7 +9077,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="17" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>73</v>
       </c>
@@ -9085,7 +9097,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>74</v>
       </c>
@@ -9102,7 +9114,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>67</v>
       </c>
@@ -9116,7 +9128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>75</v>
       </c>
@@ -9130,7 +9142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>76</v>
       </c>
@@ -9144,7 +9156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="I22" s="11" t="s">
         <v>125</v>
       </c>
@@ -9152,43 +9164,43 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F26" s="40" t="s">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="F26" s="41" t="s">
         <v>124</v>
       </c>
-      <c r="G26" s="40"/>
-      <c r="H26" s="40"/>
-      <c r="I26" s="40"/>
-      <c r="J26" s="40"/>
-      <c r="K26" s="40"/>
-      <c r="L26" s="40"/>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G26" s="41"/>
+      <c r="H26" s="41"/>
+      <c r="I26" s="41"/>
+      <c r="J26" s="41"/>
+      <c r="K26" s="41"/>
+      <c r="L26" s="41"/>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.2">
       <c r="F27" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.2">
       <c r="F28" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.2">
       <c r="F29" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.2">
       <c r="F30" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:12" x14ac:dyDescent="0.2">
       <c r="F31" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.2">
       <c r="F32" t="s">
         <v>131</v>
       </c>
@@ -9210,15 +9222,19 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEAB2FA6-8035-44D0-A545-F34162AA10FB}">
-  <dimension ref="B2:C21"/>
+  <dimension ref="B2:R22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I17" sqref="I17:J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="27" t="s">
         <v>84</v>
       </c>
@@ -9226,159 +9242,498 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>60</v>
       </c>
       <c r="C3">
         <v>135</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="F3" s="38" t="s">
+        <v>92</v>
+      </c>
+      <c r="G3" s="38"/>
+      <c r="I3" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="41"/>
+      <c r="L3" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="M3" s="41"/>
+      <c r="N3" s="41"/>
+      <c r="O3" s="41"/>
+      <c r="P3" s="41"/>
+      <c r="Q3" s="41"/>
+      <c r="R3" s="41"/>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>61</v>
       </c>
       <c r="C4">
         <v>135</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="I4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="12">
+        <f>G5</f>
+        <v>137.68421052631578</v>
+      </c>
+      <c r="L4" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="M4" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="N4" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="O4" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="P4" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q4" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="R4" s="30" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>62</v>
       </c>
       <c r="C5">
         <v>132</v>
       </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="F5" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="G5" s="10">
+        <v>137.68421052631578</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" s="2">
+        <f>G7</f>
+        <v>135</v>
+      </c>
+      <c r="L5" s="21">
+        <v>1</v>
+      </c>
+      <c r="M5" s="21">
+        <f>G14</f>
+        <v>115</v>
+      </c>
+      <c r="N5" s="29">
+        <f>M5+$J$14</f>
+        <v>135.75</v>
+      </c>
+      <c r="O5" s="21">
+        <f>(N5+M5)/2</f>
+        <v>125.375</v>
+      </c>
+      <c r="P5" s="21">
+        <v>18</v>
+      </c>
+      <c r="Q5" s="22">
+        <f>P5/$P$9</f>
+        <v>0.94736842105263153</v>
+      </c>
+      <c r="R5" s="35">
+        <f>Q5</f>
+        <v>0.94736842105263153</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>63</v>
       </c>
       <c r="C6">
         <v>137</v>
       </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="F6" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="G6" s="10">
+        <v>4.8984140120854516</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" s="1">
+        <f>G8</f>
+        <v>120</v>
+      </c>
+      <c r="L6" s="21">
+        <v>2</v>
+      </c>
+      <c r="M6" s="29">
+        <f>N5</f>
+        <v>135.75</v>
+      </c>
+      <c r="N6" s="29">
+        <f>M6+$J$14</f>
+        <v>156.5</v>
+      </c>
+      <c r="O6" s="21">
+        <f t="shared" ref="O6:O8" si="0">(N6+M6)/2</f>
+        <v>146.125</v>
+      </c>
+      <c r="P6" s="21">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="22">
+        <f t="shared" ref="Q6:Q8" si="1">P6/$P$9</f>
+        <v>0</v>
+      </c>
+      <c r="R6" s="35">
+        <f>Q6+R5</f>
+        <v>0.94736842105263153</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>64</v>
       </c>
       <c r="C7">
         <v>120</v>
       </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="F7" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="G7" s="10">
+        <v>135</v>
+      </c>
+      <c r="L7" s="21">
+        <v>3</v>
+      </c>
+      <c r="M7" s="29">
+        <f t="shared" ref="M7:M8" si="2">N6</f>
+        <v>156.5</v>
+      </c>
+      <c r="N7" s="29">
+        <f t="shared" ref="N7:N8" si="3">M7+$J$14</f>
+        <v>177.25</v>
+      </c>
+      <c r="O7" s="21">
+        <f t="shared" si="0"/>
+        <v>166.875</v>
+      </c>
+      <c r="P7" s="21">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R7" s="35">
+        <f t="shared" ref="R7:R8" si="4">Q7+R6</f>
+        <v>0.94736842105263153</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>65</v>
       </c>
       <c r="C8">
         <v>115</v>
       </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="F8" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="G8" s="10">
+        <v>120</v>
+      </c>
+      <c r="I8" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="41"/>
+      <c r="L8" s="21">
+        <v>4</v>
+      </c>
+      <c r="M8" s="29">
+        <f t="shared" si="2"/>
+        <v>177.25</v>
+      </c>
+      <c r="N8" s="29">
+        <f t="shared" si="3"/>
+        <v>198</v>
+      </c>
+      <c r="O8" s="21">
+        <f t="shared" si="0"/>
+        <v>187.625</v>
+      </c>
+      <c r="P8" s="21">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="22">
+        <f t="shared" si="1"/>
+        <v>5.2631578947368418E-2</v>
+      </c>
+      <c r="R8" s="35">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>66</v>
       </c>
       <c r="C9">
         <v>115</v>
       </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="F9" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="G9" s="10">
+        <v>21.351691662304109</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J9" s="1">
+        <f>G13</f>
+        <v>83</v>
+      </c>
+      <c r="L9" t="s">
+        <v>25</v>
+      </c>
+      <c r="P9">
+        <f>SUM(P5:P8)</f>
+        <v>19</v>
+      </c>
+      <c r="Q9" s="34">
+        <f>SUM(Q5:Q8)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>67</v>
       </c>
       <c r="C10">
         <v>120</v>
       </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="F10" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="G10" s="10">
+        <v>455.89473684210679</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J10" s="13">
+        <f>G9</f>
+        <v>21.351691662304109</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>68</v>
       </c>
       <c r="C11">
         <v>140</v>
       </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="F11" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="G11" s="10">
+        <v>2.8447768201470462</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J11" s="12">
+        <f>G10</f>
+        <v>455.89473684210679</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>70</v>
       </c>
       <c r="C12">
         <v>135</v>
       </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="F12" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="G12" s="10">
+        <v>1.600355942570429</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>69</v>
       </c>
       <c r="C13">
         <v>155</v>
       </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="F13" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="G13" s="10">
+        <v>83</v>
+      </c>
+      <c r="I13" s="39" t="s">
+        <v>106</v>
+      </c>
+      <c r="J13" s="25" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>71</v>
       </c>
       <c r="C14">
         <v>140</v>
       </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="F14" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="G14" s="10">
+        <v>115</v>
+      </c>
+      <c r="I14" s="36">
+        <f>ROUND(SQRT(G17),0)</f>
+        <v>4</v>
+      </c>
+      <c r="J14" s="13">
+        <f>G13/I14</f>
+        <v>20.75</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>72</v>
       </c>
       <c r="C15">
         <v>120</v>
       </c>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="F15" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="G15" s="10">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>68</v>
       </c>
       <c r="C16">
         <v>198</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="F16" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="G16" s="10">
+        <v>2616</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>73</v>
       </c>
       <c r="C17">
         <v>120</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="F17" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="G17" s="11">
+        <v>19</v>
+      </c>
+      <c r="I17" s="33" t="s">
+        <v>113</v>
+      </c>
+      <c r="J17" s="33" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>74</v>
       </c>
       <c r="C18">
         <v>140</v>
       </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="I18" s="32">
+        <v>135.75</v>
+      </c>
+      <c r="J18" s="10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>67</v>
       </c>
       <c r="C19">
         <v>179</v>
       </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="I19" s="32">
+        <v>156.5</v>
+      </c>
+      <c r="J19" s="10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>75</v>
       </c>
       <c r="C20">
         <v>130</v>
       </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="I20" s="32">
+        <v>177.25</v>
+      </c>
+      <c r="J20" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>76</v>
       </c>
       <c r="C21">
         <v>150</v>
       </c>
+      <c r="I21" s="32">
+        <v>198</v>
+      </c>
+      <c r="J21" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I22" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="J22" s="11">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I18:I21">
+    <sortCondition ref="I18"/>
+  </sortState>
+  <mergeCells count="3">
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="L3:R3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>